<commit_message>
to be fixed in meeting
</commit_message>
<xml_diff>
--- a/path.xlsx
+++ b/path.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F115"/>
+  <dimension ref="A1:G170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,24 +460,32 @@
           <t>Y Vel</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Yaw</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.561895</v>
+        <v>1.410944</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="D2" t="n">
-        <v>2.220446049250313e-15</v>
+        <v>8.75</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -486,18 +494,21 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.651017</v>
+        <v>1.500786</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="D3" t="n">
-        <v>2.220446049250313e-15</v>
+        <v>8.75</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -506,18 +517,21 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.725571</v>
+        <v>1.582217</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="D4" t="n">
-        <v>2.220446049250313e-15</v>
+        <v>8.75</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -526,19 +540,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1.807947</v>
+        <v>1.657208</v>
       </c>
       <c r="C5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="n">
+        <v>8.75</v>
+      </c>
+      <c r="E5" t="n">
         <v>0</v>
       </c>
-      <c r="D5" t="n">
-        <v>0.0007789230439811945</v>
-      </c>
-      <c r="E5" t="n">
-        <v>-0.002735002897679806</v>
-      </c>
       <c r="F5" t="n">
-        <v>3.636084100477888e-09</v>
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -546,19 +563,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1.884427</v>
+        <v>1.747437</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.003858566284179688</v>
+        <v>1000</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0007391357212327421</v>
+        <v>8.75</v>
       </c>
       <c r="E6" t="n">
-        <v>0.001966567477211356</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.04890589043498039</v>
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -566,19 +586,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.995825</v>
+        <v>1.82797</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.003826141357421875</v>
+        <v>1000</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0006210708525031805</v>
+        <v>8.75</v>
       </c>
       <c r="E7" t="n">
-        <v>9.069535735761747e-05</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.006419086363166571</v>
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -586,19 +609,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>2.112681</v>
+        <v>1.920707</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.003999710083007812</v>
+        <v>1000.000732421875</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0006684112595394254</v>
+        <v>8.75</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.0004444449732545763</v>
+        <v>-0.002735002897679806</v>
       </c>
       <c r="F8" t="n">
-        <v>0.01059147343039513</v>
+        <v>3.633828571381059e-09</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -606,19 +632,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>2.206136</v>
+        <v>2.00348</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.004122734069824219</v>
+        <v>1000.000732421875</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0007501601940020919</v>
+        <v>8.75</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.0004884694353677332</v>
+        <v>-0.002735002897679806</v>
       </c>
       <c r="F9" t="n">
-        <v>0.01488662697374821</v>
+        <v>3.633828571381059e-09</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -626,19 +655,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>2.316283</v>
+        <v>2.088187</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.004186630249023438</v>
+        <v>1000.000732421875</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0008752822759561241</v>
+        <v>8.74616527557373</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.0002687859814614058</v>
+        <v>0.001835593837313354</v>
       </c>
       <c r="F10" t="n">
-        <v>0.01047465577721596</v>
+        <v>-0.04869551956653595</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-0.0006713866605423391</v>
       </c>
     </row>
     <row r="11">
@@ -646,19 +678,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>2.4089</v>
+        <v>2.177559</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.004181861877441406</v>
+        <v>1000.000732421875</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0009105682256631553</v>
+        <v>8.74616527557373</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.000173598964465782</v>
+        <v>0.001835593837313354</v>
       </c>
       <c r="F11" t="n">
-        <v>0.007320110686123371</v>
+        <v>-0.04869551956653595</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-0.0006713866605423391</v>
       </c>
     </row>
     <row r="12">
@@ -666,19 +701,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>2.498715</v>
+        <v>2.262819</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.00417327880859375</v>
+        <v>1000.000549316406</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0009326171712018549</v>
+        <v>8.74620532989502</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.0001070562066161074</v>
+        <v>6.809675687691197e-05</v>
       </c>
       <c r="F12" t="n">
-        <v>0.004767397418618202</v>
+        <v>-0.006366176530718803</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-0.0007934570894576609</v>
       </c>
     </row>
     <row r="13">
@@ -686,19 +724,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>2.575785</v>
+        <v>2.341749</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.004163742065429688</v>
+        <v>1000.000549316406</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0009457015548832715</v>
+        <v>8.74620532989502</v>
       </c>
       <c r="E13" t="n">
-        <v>-6.365204899339005e-05</v>
+        <v>6.809675687691197e-05</v>
       </c>
       <c r="F13" t="n">
-        <v>0.002930273534730077</v>
+        <v>-0.006366176530718803</v>
+      </c>
+      <c r="G13" t="n">
+        <v>-0.0007934570894576609</v>
       </c>
     </row>
     <row r="14">
@@ -706,19 +747,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>2.66977</v>
+        <v>2.429823</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.00415802001953125</v>
+        <v>1000.000610351562</v>
       </c>
       <c r="D14" t="n">
-        <v>0.00095367431640625</v>
+        <v>8.746031761169434</v>
       </c>
       <c r="E14" t="n">
-        <v>-3.693102917168289e-05</v>
+        <v>-0.000417017174186185</v>
       </c>
       <c r="F14" t="n">
-        <v>0.001707602292299271</v>
+        <v>0.01056433189660311</v>
+      </c>
+      <c r="G14" t="n">
+        <v>-0.00079345703125</v>
       </c>
     </row>
     <row r="15">
@@ -726,19 +770,22 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>2.767962</v>
+        <v>2.512247</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.004183769226074219</v>
+        <v>1000.000610351562</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0009561157203279436</v>
+        <v>8.746031761169434</v>
       </c>
       <c r="E15" t="n">
-        <v>-1.049451930157375e-05</v>
+        <v>-0.000417017174186185</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0001142098190030083</v>
+        <v>0.01056433189660311</v>
+      </c>
+      <c r="G15" t="n">
+        <v>-0.00079345703125</v>
       </c>
     </row>
     <row r="16">
@@ -746,19 +793,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>2.848995</v>
+        <v>2.596804</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.004212379455566406</v>
+        <v>1000.000610351562</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0009581375052221119</v>
+        <v>8.746031761169434</v>
       </c>
       <c r="E16" t="n">
-        <v>-1.247577438334702e-05</v>
+        <v>-0.000417017174186185</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0001269933709409088</v>
+        <v>0.01056433189660311</v>
+      </c>
+      <c r="G16" t="n">
+        <v>-0.00079345703125</v>
       </c>
     </row>
     <row r="17">
@@ -766,19 +816,22 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>2.97388</v>
+        <v>2.693725</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.004238128662109375</v>
+        <v>1000.000732421875</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0009599685436114669</v>
+        <v>8.745903968811035</v>
       </c>
       <c r="E17" t="n">
-        <v>-1.015021098282887e-05</v>
+        <v>-0.0004458405310288072</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0001037191177601926</v>
+        <v>0.01482934225350618</v>
+      </c>
+      <c r="G17" t="n">
+        <v>-0.0007019041222520173</v>
       </c>
     </row>
     <row r="18">
@@ -786,19 +839,22 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>3.109178</v>
+        <v>2.777297</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.004258155822753906</v>
+        <v>1000.000732421875</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0009613037109375</v>
+        <v>8.745903968811035</v>
       </c>
       <c r="E18" t="n">
-        <v>-7.14502903065295e-06</v>
+        <v>-0.0004458405310288072</v>
       </c>
       <c r="F18" t="n">
-        <v>7.459735934389755e-05</v>
+        <v>0.01482934225350618</v>
+      </c>
+      <c r="G18" t="n">
+        <v>-0.0007019041222520173</v>
       </c>
     </row>
     <row r="19">
@@ -806,19 +862,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>3.217123</v>
+        <v>2.876399</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.0042724609375</v>
+        <v>1000.000854492188</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0009622955112718046</v>
+        <v>8.745845794677734</v>
       </c>
       <c r="E19" t="n">
-        <v>-2.715672735575936e-06</v>
+        <v>-0.0003465904155746102</v>
       </c>
       <c r="F19" t="n">
-        <v>3.036373527720571e-05</v>
+        <v>0.01352384872734547</v>
+      </c>
+      <c r="G19" t="n">
+        <v>-0.00054931640625</v>
       </c>
     </row>
     <row r="20">
@@ -826,19 +885,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>3.316771</v>
+        <v>2.96205</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.004278182983398438</v>
+        <v>1000.000854492188</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0009627532563172281</v>
+        <v>8.745845794677734</v>
       </c>
       <c r="E20" t="n">
-        <v>-2.349403985135723e-06</v>
+        <v>-0.0003465904155746102</v>
       </c>
       <c r="F20" t="n">
-        <v>2.659222263901029e-05</v>
+        <v>0.01352384872734547</v>
+      </c>
+      <c r="G20" t="n">
+        <v>-0.00054931640625</v>
       </c>
     </row>
     <row r="21">
@@ -846,19 +908,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>3.406678</v>
+        <v>3.068442</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.004281997680664062</v>
+        <v>1000.000915527344</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0009630203130654991</v>
+        <v>8.745829582214355</v>
       </c>
       <c r="E21" t="n">
-        <v>-1.638299409023602e-06</v>
+        <v>-0.0002376677002757788</v>
       </c>
       <c r="F21" t="n">
-        <v>1.986413917620666e-05</v>
+        <v>0.0104242404922843</v>
+      </c>
+      <c r="G21" t="n">
+        <v>-0.0003662109666038305</v>
       </c>
     </row>
     <row r="22">
@@ -866,19 +931,22 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>3.494944</v>
+        <v>3.166741</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.004284858703613281</v>
+        <v>1000.000915527344</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0009631347493268549</v>
+        <v>8.745829582214355</v>
       </c>
       <c r="E22" t="n">
-        <v>-3.800897161454486e-07</v>
+        <v>-0.000152517925016582</v>
       </c>
       <c r="F22" t="n">
-        <v>4.497101144806948e-06</v>
+        <v>0.007282883860170841</v>
+      </c>
+      <c r="G22" t="n">
+        <v>-0.0002136230323230848</v>
       </c>
     </row>
     <row r="23">
@@ -886,19 +954,22 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>3.62404</v>
+        <v>3.26175</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.004281997680664062</v>
+        <v>1000.0009765625</v>
       </c>
       <c r="D23" t="n">
-        <v>0.06726448237895966</v>
+        <v>8.745831489562988</v>
       </c>
       <c r="E23" t="n">
-        <v>1.256192564964294</v>
+        <v>-0.000152517925016582</v>
       </c>
       <c r="F23" t="n">
-        <v>5.074222281109542e-05</v>
+        <v>0.007282883860170841</v>
+      </c>
+      <c r="G23" t="n">
+        <v>-0.0002136230323230848</v>
       </c>
     </row>
     <row r="24">
@@ -906,19 +977,22 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>3.758589</v>
+        <v>3.359781</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.004281997680664062</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D24" t="n">
-        <v>0.2764542400836945</v>
+        <v>8.74583911895752</v>
       </c>
       <c r="E24" t="n">
-        <v>2.575804471969604</v>
+        <v>-9.406788740307093e-05</v>
       </c>
       <c r="F24" t="n">
-        <v>4.876163075095974e-05</v>
+        <v>0.004742854740470648</v>
+      </c>
+      <c r="G24" t="n">
+        <v>-0.0001220703125</v>
       </c>
     </row>
     <row r="25">
@@ -926,19 +1000,22 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>3.877632</v>
+        <v>3.44526</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.004275321960449219</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D25" t="n">
-        <v>1.023601651191711</v>
+        <v>8.74583911895752</v>
       </c>
       <c r="E25" t="n">
-        <v>4.542625427246094</v>
+        <v>-9.406788740307093e-05</v>
       </c>
       <c r="F25" t="n">
-        <v>7.04620179021731e-05</v>
+        <v>0.004742854740470648</v>
+      </c>
+      <c r="G25" t="n">
+        <v>-0.0001220703125</v>
       </c>
     </row>
     <row r="26">
@@ -946,19 +1023,22 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>3.972536</v>
+        <v>3.54241</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.004270553588867188</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D26" t="n">
-        <v>1.521474123001099</v>
+        <v>8.745846748352051</v>
       </c>
       <c r="E26" t="n">
-        <v>5.270235061645508</v>
+        <v>-5.667558434652165e-05</v>
       </c>
       <c r="F26" t="n">
-        <v>9.088518709177151e-05</v>
+        <v>0.002915197517722845</v>
+      </c>
+      <c r="G26" t="n">
+        <v>-3.05175763060106e-05</v>
       </c>
     </row>
     <row r="27">
@@ -966,19 +1046,22 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>4.060103</v>
+        <v>3.632716</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.004261016845703125</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D27" t="n">
-        <v>2.08473801612854</v>
+        <v>8.745846748352051</v>
       </c>
       <c r="E27" t="n">
-        <v>5.891059875488281</v>
+        <v>-5.667558434652165e-05</v>
       </c>
       <c r="F27" t="n">
-        <v>0.0001173404307337478</v>
+        <v>0.002915197517722845</v>
+      </c>
+      <c r="G27" t="n">
+        <v>-3.05175763060106e-05</v>
       </c>
     </row>
     <row r="28">
@@ -986,19 +1069,22 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>4.172589</v>
+        <v>3.731897</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.004250526428222656</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D28" t="n">
-        <v>2.705196857452393</v>
+        <v>8.745851516723633</v>
       </c>
       <c r="E28" t="n">
-        <v>6.438421249389648</v>
+        <v>-3.362639108672738e-05</v>
       </c>
       <c r="F28" t="n">
-        <v>0.0001475459575885907</v>
+        <v>0.001698925625532866</v>
+      </c>
+      <c r="G28" t="n">
+        <v>7.692676263104659e-06</v>
       </c>
     </row>
     <row r="29">
@@ -1006,19 +1092,22 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>4.311484</v>
+        <v>3.822532</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.004236221313476562</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D29" t="n">
-        <v>3.377372264862061</v>
+        <v>8.745851516723633</v>
       </c>
       <c r="E29" t="n">
-        <v>6.937209129333496</v>
+        <v>-3.362639108672738e-05</v>
       </c>
       <c r="F29" t="n">
-        <v>0.000182816045708023</v>
+        <v>0.001698925625532866</v>
+      </c>
+      <c r="G29" t="n">
+        <v>7.692676263104659e-06</v>
       </c>
     </row>
     <row r="30">
@@ -1026,19 +1115,22 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>4.441858</v>
+        <v>3.92075</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.004218101501464844</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D30" t="n">
-        <v>4.097573757171631</v>
+        <v>8.74582576751709</v>
       </c>
       <c r="E30" t="n">
-        <v>7.403781414031982</v>
+        <v>-1.149873605754692e-05</v>
       </c>
       <c r="F30" t="n">
-        <v>0.000222719885641709</v>
+        <v>0.0001140835447586142</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1.421349679731065e-05</v>
       </c>
     </row>
     <row r="31">
@@ -1046,19 +1138,22 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>4.564317</v>
+        <v>4.010482</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.004168510437011719</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D31" t="n">
-        <v>5.672657489776611</v>
+        <v>8.74582576751709</v>
       </c>
       <c r="E31" t="n">
-        <v>8.277637481689453</v>
+        <v>-1.149873605754692e-05</v>
       </c>
       <c r="F31" t="n">
-        <v>0.000314023724058643</v>
+        <v>0.0001140835447586142</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1.421349679731065e-05</v>
       </c>
     </row>
     <row r="32">
@@ -1066,19 +1161,22 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>4.663884</v>
+        <v>4.110848</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.004137992858886719</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D32" t="n">
-        <v>6.524415016174316</v>
+        <v>8.745797157287598</v>
       </c>
       <c r="E32" t="n">
-        <v>8.695314407348633</v>
+        <v>-1.39398889587028e-05</v>
       </c>
       <c r="F32" t="n">
-        <v>0.0003657630877569318</v>
+        <v>0.0001271224027732387</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1.427052120561711e-05</v>
       </c>
     </row>
     <row r="33">
@@ -1086,19 +1184,22 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>4.762129</v>
+        <v>4.207393</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.004100799560546875</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D33" t="n">
-        <v>7.417513847351074</v>
+        <v>8.745797157287598</v>
       </c>
       <c r="E33" t="n">
-        <v>9.103967666625977</v>
+        <v>-1.39398889587028e-05</v>
       </c>
       <c r="F33" t="n">
-        <v>0.0004234457737766206</v>
+        <v>0.0001271224027732387</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1.427052120561711e-05</v>
       </c>
     </row>
     <row r="34">
@@ -1106,19 +1207,22 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>4.867889</v>
+        <v>4.308074</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.004057884216308594</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D34" t="n">
-        <v>8.351119041442871</v>
+        <v>8.745771408081055</v>
       </c>
       <c r="E34" t="n">
-        <v>9.50516414642334</v>
+        <v>-1.134508147515589e-05</v>
       </c>
       <c r="F34" t="n">
-        <v>0.0004819101595785469</v>
+        <v>0.000103889760794118</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1.43187880894402e-05</v>
       </c>
     </row>
     <row r="35">
@@ -1126,19 +1230,22 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>5.005247</v>
+        <v>4.407125</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.004009246826171875</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D35" t="n">
-        <v>9.324525833129883</v>
+        <v>8.745771408081055</v>
       </c>
       <c r="E35" t="n">
-        <v>9.899908065795898</v>
+        <v>-1.134508147515589e-05</v>
       </c>
       <c r="F35" t="n">
-        <v>0.0005450561293400824</v>
+        <v>0.000103889760794118</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1.43187880894402e-05</v>
       </c>
     </row>
     <row r="36">
@@ -1146,19 +1253,22 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>5.132894</v>
+        <v>4.520879</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.0038909912109375</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D36" t="n">
-        <v>11.38830375671387</v>
+        <v>8.74575138092041</v>
       </c>
       <c r="E36" t="n">
-        <v>10.67243957519531</v>
+        <v>-7.979348993103486e-06</v>
       </c>
       <c r="F36" t="n">
-        <v>0.0006817218963988125</v>
+        <v>7.483115768991411e-05</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1.435257399862166e-05</v>
       </c>
     </row>
     <row r="37">
@@ -1166,19 +1276,22 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>5.240091</v>
+        <v>4.620603</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.003821372985839844</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D37" t="n">
-        <v>12.47758388519287</v>
+        <v>8.74575138092041</v>
       </c>
       <c r="E37" t="n">
-        <v>11.05096530914307</v>
+        <v>-7.979348993103486e-06</v>
       </c>
       <c r="F37" t="n">
-        <v>0.0007552294409833848</v>
+        <v>7.483115768991411e-05</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1.435257399862166e-05</v>
       </c>
     </row>
     <row r="38">
@@ -1186,19 +1299,22 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>5.351282</v>
+        <v>4.722876</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.003745079040527344</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D38" t="n">
-        <v>13.60444831848145</v>
+        <v>8.745742797851562</v>
       </c>
       <c r="E38" t="n">
-        <v>11.42464160919189</v>
+        <v>-2.142563971574418e-06</v>
       </c>
       <c r="F38" t="n">
-        <v>0.0008342734072357416</v>
+        <v>2.11067217605887e-05</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1.43694687722018e-05</v>
       </c>
     </row>
     <row r="39">
@@ -1206,19 +1322,22 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>5.480214</v>
+        <v>4.827976</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.003660202026367188</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D39" t="n">
-        <v>14.76841640472412</v>
+        <v>8.74573802947998</v>
       </c>
       <c r="E39" t="n">
-        <v>11.7936315536499</v>
+        <v>-3.128575372102205e-06</v>
       </c>
       <c r="F39" t="n">
-        <v>0.0009134497959166765</v>
+        <v>3.031447158718947e-05</v>
+      </c>
+      <c r="G39" t="n">
+        <v>1.438458093616646e-05</v>
       </c>
     </row>
     <row r="40">
@@ -1226,19 +1345,22 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>5.61414</v>
+        <v>4.926635</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.003464698791503906</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D40" t="n">
-        <v>17.20582008361816</v>
+        <v>8.74573802947998</v>
       </c>
       <c r="E40" t="n">
-        <v>12.51799297332764</v>
+        <v>-3.128575372102205e-06</v>
       </c>
       <c r="F40" t="n">
-        <v>0.001082889270037413</v>
+        <v>3.031447158718947e-05</v>
+      </c>
+      <c r="G40" t="n">
+        <v>1.438458093616646e-05</v>
       </c>
     </row>
     <row r="41">
@@ -1246,19 +1368,22 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>5.730177</v>
+        <v>5.02935</v>
       </c>
       <c r="C41" t="n">
-        <v>-0.003354072570800781</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D41" t="n">
-        <v>18.47835731506348</v>
+        <v>8.745732307434082</v>
       </c>
       <c r="E41" t="n">
-        <v>12.87354373931885</v>
+        <v>-2.649436510182568e-06</v>
       </c>
       <c r="F41" t="n">
-        <v>0.001172156305983663</v>
+        <v>2.660348218341824e-05</v>
+      </c>
+      <c r="G41" t="n">
+        <v>1.439588504581479e-05</v>
       </c>
     </row>
     <row r="42">
@@ -1266,19 +1391,22 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>5.873293</v>
+        <v>5.131444</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.00323486328125</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D42" t="n">
-        <v>19.78619956970215</v>
+        <v>8.745732307434082</v>
       </c>
       <c r="E42" t="n">
-        <v>13.22477531433105</v>
+        <v>-2.649436510182568e-06</v>
       </c>
       <c r="F42" t="n">
-        <v>0.001265974598936737</v>
+        <v>2.660348218341824e-05</v>
+      </c>
+      <c r="G42" t="n">
+        <v>1.439588504581479e-05</v>
       </c>
     </row>
     <row r="43">
@@ -1286,19 +1414,22 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>6.01524</v>
+        <v>5.249266</v>
       </c>
       <c r="C43" t="n">
-        <v>-0.003106117248535156</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D43" t="n">
-        <v>21.12891960144043</v>
+        <v>8.7457275390625</v>
       </c>
       <c r="E43" t="n">
-        <v>13.57175064086914</v>
+        <v>-1.935645514095086e-06</v>
       </c>
       <c r="F43" t="n">
-        <v>0.001360558439046144</v>
+        <v>1.994365993596148e-05</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1.440321375412168e-05</v>
       </c>
     </row>
     <row r="44">
@@ -1306,19 +1437,22 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>6.137888</v>
+        <v>5.354506</v>
       </c>
       <c r="C44" t="n">
-        <v>-0.002818107604980469</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D44" t="n">
-        <v>23.91730880737305</v>
+        <v>8.7457275390625</v>
       </c>
       <c r="E44" t="n">
-        <v>14.25316333770752</v>
+        <v>-1.935645514095086e-06</v>
       </c>
       <c r="F44" t="n">
-        <v>0.001560292672365904</v>
+        <v>1.994365993596148e-05</v>
+      </c>
+      <c r="G44" t="n">
+        <v>1.440321375412168e-05</v>
       </c>
     </row>
     <row r="45">
@@ -1326,19 +1460,22 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>6.256346</v>
+        <v>5.461165</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.002657890319824219</v>
+        <v>1000.001098632812</v>
       </c>
       <c r="D45" t="n">
-        <v>25.36214828491211</v>
+        <v>8.745724678039551</v>
       </c>
       <c r="E45" t="n">
-        <v>14.58770847320557</v>
+        <v>-4.014884495973092e-07</v>
       </c>
       <c r="F45" t="n">
-        <v>0.001665810937993228</v>
+        <v>4.645531589630991e-06</v>
+      </c>
+      <c r="G45" t="n">
+        <v>1.440676714992151e-05</v>
       </c>
     </row>
     <row r="46">
@@ -1346,19 +1483,22 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>6.36997</v>
+        <v>5.568505</v>
       </c>
       <c r="C46" t="n">
-        <v>-0.002489089965820312</v>
+        <v>1000.0673828125</v>
       </c>
       <c r="D46" t="n">
-        <v>26.8402099609375</v>
+        <v>8.745007514953613</v>
       </c>
       <c r="E46" t="n">
-        <v>14.91821098327637</v>
+        <v>1.255920052528381</v>
       </c>
       <c r="F46" t="n">
-        <v>0.001774050528183579</v>
+        <v>-0.01732652448117733</v>
+      </c>
+      <c r="G46" t="n">
+        <v>-0.02642822265625</v>
       </c>
     </row>
     <row r="47">
@@ -1366,19 +1506,22 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>6.518429</v>
+        <v>5.674587</v>
       </c>
       <c r="C47" t="n">
-        <v>-0.002308845520019531</v>
+        <v>1000.0673828125</v>
       </c>
       <c r="D47" t="n">
-        <v>28.3510913848877</v>
+        <v>8.745007514953613</v>
       </c>
       <c r="E47" t="n">
-        <v>15.24472522735596</v>
+        <v>1.255920052528381</v>
       </c>
       <c r="F47" t="n">
-        <v>0.001886782934889197</v>
+        <v>-0.01732652448117733</v>
+      </c>
+      <c r="G47" t="n">
+        <v>-0.02642822265625</v>
       </c>
     </row>
     <row r="48">
@@ -1386,19 +1529,22 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>6.657033</v>
+        <v>5.793779</v>
       </c>
       <c r="C48" t="n">
-        <v>-0.001920700073242188</v>
+        <v>1000.276489257812</v>
       </c>
       <c r="D48" t="n">
-        <v>31.46972274780273</v>
+        <v>8.742654800415039</v>
       </c>
       <c r="E48" t="n">
-        <v>15.88596725463867</v>
+        <v>2.575202941894531</v>
       </c>
       <c r="F48" t="n">
-        <v>0.001975540770217776</v>
+        <v>-0.03915747255086899</v>
+      </c>
+      <c r="G48" t="n">
+        <v>-0.1107788011431694</v>
       </c>
     </row>
     <row r="49">
@@ -1406,19 +1552,22 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>6.776653</v>
+        <v>5.901219</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.001722335815429688</v>
+        <v>1000.276489257812</v>
       </c>
       <c r="D49" t="n">
-        <v>33.07669448852539</v>
+        <v>8.742654800415039</v>
       </c>
       <c r="E49" t="n">
-        <v>16.2007884979248</v>
+        <v>2.575202941894531</v>
       </c>
       <c r="F49" t="n">
-        <v>0.001971280435100198</v>
+        <v>-0.03915747255086899</v>
+      </c>
+      <c r="G49" t="n">
+        <v>-0.1107788011431694</v>
       </c>
     </row>
     <row r="50">
@@ -1426,19 +1575,22 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>6.90828</v>
+        <v>6.007678</v>
       </c>
       <c r="C50" t="n">
-        <v>-0.001523971557617188</v>
+        <v>1000.602661132812</v>
       </c>
       <c r="D50" t="n">
-        <v>34.71493148803711</v>
+        <v>8.738525390625</v>
       </c>
       <c r="E50" t="n">
-        <v>16.51180839538574</v>
+        <v>3.662173748016357</v>
       </c>
       <c r="F50" t="n">
-        <v>0.001948837889358401</v>
+        <v>-0.06300290673971176</v>
+      </c>
+      <c r="G50" t="n">
+        <v>-0.2413635551929474</v>
       </c>
     </row>
     <row r="51">
@@ -1446,19 +1598,22 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>7.051165</v>
+        <v>6.118115</v>
       </c>
       <c r="C51" t="n">
-        <v>-0.001142501831054688</v>
+        <v>1001.023254394531</v>
       </c>
       <c r="D51" t="n">
-        <v>38.08368301391602</v>
+        <v>8.732319831848145</v>
       </c>
       <c r="E51" t="n">
-        <v>17.12260627746582</v>
+        <v>4.541271209716797</v>
       </c>
       <c r="F51" t="n">
-        <v>0.001819510711356997</v>
+        <v>-0.08916348963975906</v>
+      </c>
+      <c r="G51" t="n">
+        <v>-0.4074401259422302</v>
       </c>
     </row>
     <row r="52">
@@ -1466,19 +1621,22 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>7.159607</v>
+        <v>6.226041</v>
       </c>
       <c r="C52" t="n">
-        <v>-0.0009622573852539062</v>
+        <v>1001.023254394531</v>
       </c>
       <c r="D52" t="n">
-        <v>39.81344985961914</v>
+        <v>8.732319831848145</v>
       </c>
       <c r="E52" t="n">
-        <v>17.42247772216797</v>
+        <v>4.541271209716797</v>
       </c>
       <c r="F52" t="n">
-        <v>0.001734184450469911</v>
+        <v>-0.08916348963975906</v>
+      </c>
+      <c r="G52" t="n">
+        <v>-0.4074401259422302</v>
       </c>
     </row>
     <row r="53">
@@ -1486,19 +1644,22 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>7.275756</v>
+        <v>6.348738</v>
       </c>
       <c r="C53" t="n">
-        <v>-0.000789642333984375</v>
+        <v>1001.52099609375</v>
       </c>
       <c r="D53" t="n">
-        <v>41.572998046875</v>
+        <v>8.723714828491211</v>
       </c>
       <c r="E53" t="n">
-        <v>17.71872329711914</v>
+        <v>5.268417835235596</v>
       </c>
       <c r="F53" t="n">
-        <v>0.001636374508962035</v>
+        <v>-0.1172889024019241</v>
+      </c>
+      <c r="G53" t="n">
+        <v>-0.5984190702438354</v>
       </c>
     </row>
     <row r="54">
@@ -1506,19 +1667,22 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>7.406649</v>
+        <v>6.461931</v>
       </c>
       <c r="C54" t="n">
-        <v>-0.0006284713745117188</v>
+        <v>1002.083984375</v>
       </c>
       <c r="D54" t="n">
-        <v>43.36196517944336</v>
+        <v>8.712429046630859</v>
       </c>
       <c r="E54" t="n">
-        <v>18.01154899597168</v>
+        <v>5.888685703277588</v>
       </c>
       <c r="F54" t="n">
-        <v>0.001537338015623391</v>
+        <v>-0.147413432598114</v>
+      </c>
+      <c r="G54" t="n">
+        <v>-0.80487060546875</v>
       </c>
     </row>
     <row r="55">
@@ -1526,19 +1690,22 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>7.561181</v>
+        <v>6.569616</v>
       </c>
       <c r="C55" t="n">
-        <v>-0.000335693359375</v>
+        <v>1002.083984375</v>
       </c>
       <c r="D55" t="n">
-        <v>47.02693557739258</v>
+        <v>8.712429046630859</v>
       </c>
       <c r="E55" t="n">
-        <v>18.58843612670898</v>
+        <v>5.888685703277588</v>
       </c>
       <c r="F55" t="n">
-        <v>0.001330394763499498</v>
+        <v>-0.147413432598114</v>
+      </c>
+      <c r="G55" t="n">
+        <v>-0.80487060546875</v>
       </c>
     </row>
     <row r="56">
@@ -1546,19 +1713,22 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>7.688407</v>
+        <v>6.683552</v>
       </c>
       <c r="C56" t="n">
-        <v>-0.0002040863037109375</v>
+        <v>1002.704223632812</v>
       </c>
       <c r="D56" t="n">
-        <v>48.90240097045898</v>
+        <v>8.698147773742676</v>
       </c>
       <c r="E56" t="n">
-        <v>18.87305068969727</v>
+        <v>6.435371398925781</v>
       </c>
       <c r="F56" t="n">
-        <v>0.001226962893269956</v>
+        <v>-0.179594874382019</v>
+      </c>
+      <c r="G56" t="n">
+        <v>-1.01989734172821</v>
       </c>
     </row>
     <row r="57">
@@ -1566,19 +1736,22 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>7.826122</v>
+        <v>6.799497</v>
       </c>
       <c r="C57" t="n">
-        <v>-8.296966552734375e-05</v>
+        <v>1002.704223632812</v>
       </c>
       <c r="D57" t="n">
-        <v>50.80620193481445</v>
+        <v>8.698147773742676</v>
       </c>
       <c r="E57" t="n">
-        <v>19.15538215637207</v>
+        <v>6.435371398925781</v>
       </c>
       <c r="F57" t="n">
-        <v>0.001119980006478727</v>
+        <v>-0.179594874382019</v>
+      </c>
+      <c r="G57" t="n">
+        <v>-1.01989734172821</v>
       </c>
     </row>
     <row r="58">
@@ -1586,19 +1759,22 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>7.976842</v>
+        <v>6.915962</v>
       </c>
       <c r="C58" t="n">
-        <v>0.0001268386840820312</v>
+        <v>1003.376098632812</v>
       </c>
       <c r="D58" t="n">
-        <v>54.69791793823242</v>
+        <v>8.680624961853027</v>
       </c>
       <c r="E58" t="n">
-        <v>19.7137622833252</v>
+        <v>6.93337345123291</v>
       </c>
       <c r="F58" t="n">
-        <v>0.0009191785356961191</v>
+        <v>-0.2133295983076096</v>
+      </c>
+      <c r="G58" t="n">
+        <v>-1.237701296806335</v>
       </c>
     </row>
     <row r="59">
@@ -1606,19 +1782,22 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>8.096117</v>
+        <v>7.0299</v>
       </c>
       <c r="C59" t="n">
-        <v>0.0002164840698242188</v>
+        <v>1004.095825195312</v>
       </c>
       <c r="D59" t="n">
-        <v>56.68544006347656</v>
+        <v>8.659655570983887</v>
       </c>
       <c r="E59" t="n">
-        <v>19.99001502990723</v>
+        <v>7.399051189422607</v>
       </c>
       <c r="F59" t="n">
-        <v>0.0008203177712857723</v>
+        <v>-0.2483720332384109</v>
+      </c>
+      <c r="G59" t="n">
+        <v>-1.45318615436554</v>
       </c>
     </row>
     <row r="60">
@@ -1626,19 +1805,22 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>8.228498</v>
+        <v>7.148656</v>
       </c>
       <c r="C60" t="n">
-        <v>0.0002965927124023438</v>
+        <v>1004.095825195312</v>
       </c>
       <c r="D60" t="n">
-        <v>58.70047760009766</v>
+        <v>8.659655570983887</v>
       </c>
       <c r="E60" t="n">
-        <v>20.2644100189209</v>
+        <v>7.399051189422607</v>
       </c>
       <c r="F60" t="n">
-        <v>0.0007200710824690759</v>
+        <v>-0.2483720332384109</v>
+      </c>
+      <c r="G60" t="n">
+        <v>-1.45318615436554</v>
       </c>
     </row>
     <row r="61">
@@ -1646,19 +1828,22 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>8.385236000000001</v>
+        <v>7.272551</v>
       </c>
       <c r="C61" t="n">
-        <v>0.0003652572631835938</v>
+        <v>1004.861145019531</v>
       </c>
       <c r="D61" t="n">
-        <v>60.74285507202148</v>
+        <v>8.635075569152832</v>
       </c>
       <c r="E61" t="n">
-        <v>20.53700637817383</v>
+        <v>7.842730522155762</v>
       </c>
       <c r="F61" t="n">
-        <v>0.0006241864757612348</v>
+        <v>-0.2844030559062958</v>
+      </c>
+      <c r="G61" t="n">
+        <v>-1.662323236465454</v>
       </c>
     </row>
     <row r="62">
@@ -1666,19 +1851,22 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>8.516415</v>
+        <v>7.388838</v>
       </c>
       <c r="C62" t="n">
-        <v>0.000476837158203125</v>
+        <v>1005.669921875</v>
       </c>
       <c r="D62" t="n">
-        <v>64.90891265869141</v>
+        <v>8.606767654418945</v>
       </c>
       <c r="E62" t="n">
-        <v>21.07697296142578</v>
+        <v>8.270839691162109</v>
       </c>
       <c r="F62" t="n">
-        <v>0.0004314767720643431</v>
+        <v>-0.321064680814743</v>
+      </c>
+      <c r="G62" t="n">
+        <v>-1.861785650253296</v>
       </c>
     </row>
     <row r="63">
@@ -1686,19 +1874,22 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>8.649504</v>
+        <v>7.506086</v>
       </c>
       <c r="C63" t="n">
-        <v>0.0005168914794921875</v>
+        <v>1005.669921875</v>
       </c>
       <c r="D63" t="n">
-        <v>67.03224182128906</v>
+        <v>8.606767654418945</v>
       </c>
       <c r="E63" t="n">
-        <v>21.34441757202148</v>
+        <v>8.270839691162109</v>
       </c>
       <c r="F63" t="n">
-        <v>0.0003344329888932407</v>
+        <v>-0.321064680814743</v>
+      </c>
+      <c r="G63" t="n">
+        <v>-1.861785650253296</v>
       </c>
     </row>
     <row r="64">
@@ -1706,19 +1897,22 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>8.805364000000001</v>
+        <v>7.634204</v>
       </c>
       <c r="C64" t="n">
-        <v>0.0005474090576171875</v>
+        <v>1006.520812988281</v>
       </c>
       <c r="D64" t="n">
-        <v>69.18222808837891</v>
+        <v>8.574660301208496</v>
       </c>
       <c r="E64" t="n">
-        <v>21.61021041870117</v>
+        <v>8.687372207641602</v>
       </c>
       <c r="F64" t="n">
-        <v>0.000235639774473384</v>
+        <v>-0.3579919040203094</v>
+      </c>
+      <c r="G64" t="n">
+        <v>-2.049072504043579</v>
       </c>
     </row>
     <row r="65">
@@ -1726,19 +1920,22 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>8.967492</v>
+        <v>7.755283</v>
       </c>
       <c r="C65" t="n">
-        <v>0.0005788803100585938</v>
+        <v>1007.413208007812</v>
       </c>
       <c r="D65" t="n">
-        <v>73.56148529052734</v>
+        <v>8.538722038269043</v>
       </c>
       <c r="E65" t="n">
-        <v>22.13690376281738</v>
+        <v>9.094834327697754</v>
       </c>
       <c r="F65" t="n">
-        <v>2.523781222407706e-05</v>
+        <v>-0.3948204219341278</v>
+      </c>
+      <c r="G65" t="n">
+        <v>-2.2222900390625</v>
       </c>
     </row>
     <row r="66">
@@ -1746,19 +1943,22 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>9.100002</v>
+        <v>7.87917</v>
       </c>
       <c r="C66" t="n">
-        <v>0.000579833984375</v>
+        <v>1007.413208007812</v>
       </c>
       <c r="D66" t="n">
-        <v>75.79045104980469</v>
+        <v>8.538722038269043</v>
       </c>
       <c r="E66" t="n">
-        <v>22.39783668518066</v>
+        <v>9.094834327697754</v>
       </c>
       <c r="F66" t="n">
-        <v>-4.980519588571042e-05</v>
+        <v>-0.3948204219341278</v>
+      </c>
+      <c r="G66" t="n">
+        <v>-2.2222900390625</v>
       </c>
     </row>
     <row r="67">
@@ -1766,19 +1966,22 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>9.251486</v>
+        <v>8.006342</v>
       </c>
       <c r="C67" t="n">
-        <v>0.0005731582641601562</v>
+        <v>1008.345825195312</v>
       </c>
       <c r="D67" t="n">
-        <v>78.04540252685547</v>
+        <v>8.498969078063965</v>
       </c>
       <c r="E67" t="n">
-        <v>22.65718269348145</v>
+        <v>9.494812965393066</v>
       </c>
       <c r="F67" t="n">
-        <v>-0.000130672226077877</v>
+        <v>-0.431205689907074</v>
+      </c>
+      <c r="G67" t="n">
+        <v>-2.380157232284546</v>
       </c>
     </row>
     <row r="68">
@@ -1786,19 +1989,22 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>9.379458</v>
+        <v>8.126621999999999</v>
       </c>
       <c r="C68" t="n">
-        <v>0.0005369186401367188</v>
+        <v>1009.318359375</v>
       </c>
       <c r="D68" t="n">
-        <v>82.6326904296875</v>
+        <v>8.455451965332031</v>
       </c>
       <c r="E68" t="n">
-        <v>23.17116165161133</v>
+        <v>9.888334274291992</v>
       </c>
       <c r="F68" t="n">
-        <v>-0.0002522591967135668</v>
+        <v>-0.4668321907520294</v>
+      </c>
+      <c r="G68" t="n">
+        <v>-2.521850347518921</v>
       </c>
     </row>
     <row r="69">
@@ -1806,19 +2012,22 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>9.518212</v>
+        <v>8.249185000000001</v>
       </c>
       <c r="C69" t="n">
-        <v>0.0005102157592773438</v>
+        <v>1009.318359375</v>
       </c>
       <c r="D69" t="n">
-        <v>84.96470642089844</v>
+        <v>8.455451965332031</v>
       </c>
       <c r="E69" t="n">
-        <v>23.42581939697266</v>
+        <v>9.888334274291992</v>
       </c>
       <c r="F69" t="n">
-        <v>-0.0002972972870338708</v>
+        <v>-0.4668321907520294</v>
+      </c>
+      <c r="G69" t="n">
+        <v>-2.521850347518921</v>
       </c>
     </row>
     <row r="70">
@@ -1826,19 +2035,22 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>9.658497000000001</v>
+        <v>8.373848000000001</v>
       </c>
       <c r="C70" t="n">
-        <v>0.0004796981811523438</v>
+        <v>1010.329772949219</v>
       </c>
       <c r="D70" t="n">
-        <v>87.32209777832031</v>
+        <v>8.408257484436035</v>
       </c>
       <c r="E70" t="n">
-        <v>23.67893218994141</v>
+        <v>10.27607440948486</v>
       </c>
       <c r="F70" t="n">
-        <v>-0.0003349915496073663</v>
+        <v>-0.5014278888702393</v>
+      </c>
+      <c r="G70" t="n">
+        <v>-2.647094488143921</v>
       </c>
     </row>
     <row r="71">
@@ -1846,19 +2058,22 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>9.812231000000001</v>
+        <v>8.493789</v>
       </c>
       <c r="C71" t="n">
-        <v>0.0004091262817382812</v>
+        <v>1011.379638671875</v>
       </c>
       <c r="D71" t="n">
-        <v>92.11240386962891</v>
+        <v>8.357501983642578</v>
       </c>
       <c r="E71" t="n">
-        <v>24.18057632446289</v>
+        <v>10.65848731994629</v>
       </c>
       <c r="F71" t="n">
-        <v>-0.0003815666423179209</v>
+        <v>-0.5347641110420227</v>
+      </c>
+      <c r="G71" t="n">
+        <v>-2.756012439727783</v>
       </c>
     </row>
     <row r="72">
@@ -1866,19 +2081,22 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>9.955997999999999</v>
+        <v>8.620566</v>
       </c>
       <c r="C72" t="n">
-        <v>0.000370025634765625</v>
+        <v>1011.379638671875</v>
       </c>
       <c r="D72" t="n">
-        <v>94.54499816894531</v>
+        <v>8.357501983642578</v>
       </c>
       <c r="E72" t="n">
-        <v>24.42911720275879</v>
+        <v>10.65848731994629</v>
       </c>
       <c r="F72" t="n">
-        <v>-0.0003960801695939153</v>
+        <v>-0.5347641110420227</v>
+      </c>
+      <c r="G72" t="n">
+        <v>-2.756012439727783</v>
       </c>
     </row>
     <row r="73">
@@ -1886,19 +2104,22 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>10.100131</v>
+        <v>8.743520999999999</v>
       </c>
       <c r="C73" t="n">
-        <v>0.0003309249877929688</v>
+        <v>1012.467468261719</v>
       </c>
       <c r="D73" t="n">
-        <v>97.00238037109375</v>
+        <v>8.303324699401855</v>
       </c>
       <c r="E73" t="n">
-        <v>24.67615699768066</v>
+        <v>11.03588962554932</v>
       </c>
       <c r="F73" t="n">
-        <v>-0.0004067272529937327</v>
+        <v>-0.5666682720184326</v>
+      </c>
+      <c r="G73" t="n">
+        <v>-2.849059820175171</v>
       </c>
     </row>
     <row r="74">
@@ -1906,19 +2127,22 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>10.259237</v>
+        <v>8.869906</v>
       </c>
       <c r="C74" t="n">
-        <v>0.0002508163452148438</v>
+        <v>1013.592895507812</v>
       </c>
       <c r="D74" t="n">
-        <v>101.9908065795898</v>
+        <v>8.245881080627441</v>
       </c>
       <c r="E74" t="n">
-        <v>25.16574478149414</v>
+        <v>11.40850639343262</v>
       </c>
       <c r="F74" t="n">
-        <v>-0.0004165362915955484</v>
+        <v>-0.5970171093940735</v>
+      </c>
+      <c r="G74" t="n">
+        <v>-2.927033424377441</v>
       </c>
     </row>
     <row r="75">
@@ -1926,19 +2150,22 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>10.402939</v>
+        <v>9.002128000000001</v>
       </c>
       <c r="C75" t="n">
-        <v>0.0002107620239257812</v>
+        <v>1014.755065917969</v>
       </c>
       <c r="D75" t="n">
-        <v>104.521598815918</v>
+        <v>8.185341835021973</v>
       </c>
       <c r="E75" t="n">
-        <v>25.40830993652344</v>
+        <v>11.77649974822998</v>
       </c>
       <c r="F75" t="n">
-        <v>-0.000418086041463539</v>
+        <v>-0.6257410049438477</v>
+      </c>
+      <c r="G75" t="n">
+        <v>-2.990967273712158</v>
       </c>
     </row>
     <row r="76">
@@ -1946,19 +2173,22 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>10.559696</v>
+        <v>9.122585000000001</v>
       </c>
       <c r="C76" t="n">
-        <v>0.00012969970703125</v>
+        <v>1014.755065917969</v>
       </c>
       <c r="D76" t="n">
-        <v>109.6555023193359</v>
+        <v>8.185341835021973</v>
       </c>
       <c r="E76" t="n">
-        <v>25.88901710510254</v>
+        <v>11.77649974822998</v>
       </c>
       <c r="F76" t="n">
-        <v>-0.0004163784324191511</v>
+        <v>-0.6257410049438477</v>
+      </c>
+      <c r="G76" t="n">
+        <v>-2.990967273712158</v>
       </c>
     </row>
     <row r="77">
@@ -1966,19 +2196,22 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>10.717115</v>
+        <v>9.259536000000001</v>
       </c>
       <c r="C77" t="n">
-        <v>8.96453857421875e-05</v>
+        <v>1015.953857421875</v>
       </c>
       <c r="D77" t="n">
-        <v>112.2583465576172</v>
+        <v>8.121878623962402</v>
       </c>
       <c r="E77" t="n">
-        <v>26.12717437744141</v>
+        <v>12.13999938964844</v>
       </c>
       <c r="F77" t="n">
-        <v>-0.0004135965136811137</v>
+        <v>-0.6528212428092957</v>
+      </c>
+      <c r="G77" t="n">
+        <v>-3.042053461074829</v>
       </c>
     </row>
     <row r="78">
@@ -1986,19 +2219,22 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>10.878868</v>
+        <v>9.386742</v>
       </c>
       <c r="C78" t="n">
-        <v>8.58306884765625e-06</v>
+        <v>1017.188903808594</v>
       </c>
       <c r="D78" t="n">
-        <v>117.5350875854492</v>
+        <v>8.055670738220215</v>
       </c>
       <c r="E78" t="n">
-        <v>26.5991325378418</v>
+        <v>12.49910449981689</v>
       </c>
       <c r="F78" t="n">
-        <v>-0.0004052480217069387</v>
+        <v>-0.6782829761505127</v>
+      </c>
+      <c r="G78" t="n">
+        <v>-3.081635475158691</v>
       </c>
     </row>
     <row r="79">
@@ -2006,19 +2242,22 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>11.037201</v>
+        <v>9.517325</v>
       </c>
       <c r="C79" t="n">
-        <v>-3.147125244140625e-05</v>
+        <v>1017.188903808594</v>
       </c>
       <c r="D79" t="n">
-        <v>120.2086791992188</v>
+        <v>8.055670738220215</v>
       </c>
       <c r="E79" t="n">
-        <v>26.83294868469238</v>
+        <v>12.49910449981689</v>
       </c>
       <c r="F79" t="n">
-        <v>-0.0003871879016514868</v>
+        <v>-0.6782829761505127</v>
+      </c>
+      <c r="G79" t="n">
+        <v>-3.081635475158691</v>
       </c>
     </row>
     <row r="80">
@@ -2026,19 +2265,22 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>11.202866</v>
+        <v>9.646459999999999</v>
       </c>
       <c r="C80" t="n">
-        <v>-0.0001049041748046875</v>
+        <v>1018.459533691406</v>
       </c>
       <c r="D80" t="n">
-        <v>125.6256256103516</v>
+        <v>7.986887454986572</v>
       </c>
       <c r="E80" t="n">
-        <v>27.29627799987793</v>
+        <v>12.8538932800293</v>
       </c>
       <c r="F80" t="n">
-        <v>-0.0003423873567953706</v>
+        <v>-0.7021879553794861</v>
+      </c>
+      <c r="G80" t="n">
+        <v>-3.111083984375</v>
       </c>
     </row>
     <row r="81">
@@ -2046,19 +2288,22 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>11.340403</v>
+        <v>9.777232</v>
       </c>
       <c r="C81" t="n">
-        <v>-0.0001382827758789062</v>
+        <v>1019.765380859375</v>
       </c>
       <c r="D81" t="n">
-        <v>128.3686828613281</v>
+        <v>7.915695667266846</v>
       </c>
       <c r="E81" t="n">
-        <v>27.52581787109375</v>
+        <v>13.20443344116211</v>
       </c>
       <c r="F81" t="n">
-        <v>-0.000310924369841814</v>
+        <v>-0.7246329188346863</v>
+      </c>
+      <c r="G81" t="n">
+        <v>-3.131836652755737</v>
       </c>
     </row>
     <row r="82">
@@ -2066,19 +2311,22 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>11.514668</v>
+        <v>9.909305</v>
       </c>
       <c r="C82" t="n">
-        <v>-0.0001926422119140625</v>
+        <v>1021.106079101562</v>
       </c>
       <c r="D82" t="n">
-        <v>133.9232940673828</v>
+        <v>7.842248439788818</v>
       </c>
       <c r="E82" t="n">
-        <v>27.98065948486328</v>
+        <v>13.55078220367432</v>
       </c>
       <c r="F82" t="n">
-        <v>-0.0002331276918994263</v>
+        <v>-0.7457382082939148</v>
+      </c>
+      <c r="G82" t="n">
+        <v>-3.14532470703125</v>
       </c>
     </row>
     <row r="83">
@@ -2086,19 +2334,22 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>11.656452</v>
+        <v>10.038221</v>
       </c>
       <c r="C83" t="n">
-        <v>-0.0002145767211914062</v>
+        <v>1021.106079101562</v>
       </c>
       <c r="D83" t="n">
-        <v>136.7345428466797</v>
+        <v>7.842248439788818</v>
       </c>
       <c r="E83" t="n">
-        <v>28.20597648620605</v>
+        <v>13.55078220367432</v>
       </c>
       <c r="F83" t="n">
-        <v>-0.0001885885722003877</v>
+        <v>-0.7457382082939148</v>
+      </c>
+      <c r="G83" t="n">
+        <v>-3.14532470703125</v>
       </c>
     </row>
     <row r="84">
@@ -2106,19 +2357,22 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>11.827123</v>
+        <v>10.175218</v>
       </c>
       <c r="C84" t="n">
-        <v>-0.0002317428588867188</v>
+        <v>1022.481140136719</v>
       </c>
       <c r="D84" t="n">
-        <v>139.5682525634766</v>
+        <v>7.766683578491211</v>
       </c>
       <c r="E84" t="n">
-        <v>28.42990493774414</v>
+        <v>13.89299011230469</v>
       </c>
       <c r="F84" t="n">
-        <v>-0.0001410992263117805</v>
+        <v>-0.7656408548355103</v>
+      </c>
+      <c r="G84" t="n">
+        <v>-3.152801513671875</v>
       </c>
     </row>
     <row r="85">
@@ -2126,19 +2380,22 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>12.00213</v>
+        <v>10.308876</v>
       </c>
       <c r="C85" t="n">
-        <v>-0.0002527236938476562</v>
+        <v>1023.89013671875</v>
       </c>
       <c r="D85" t="n">
-        <v>145.302490234375</v>
+        <v>7.689128398895264</v>
       </c>
       <c r="E85" t="n">
-        <v>28.87360382080078</v>
+        <v>14.23110675811768</v>
       </c>
       <c r="F85" t="n">
-        <v>-4.202354466542602e-05</v>
+        <v>-0.7844861149787903</v>
+      </c>
+      <c r="G85" t="n">
+        <v>-3.155549049377441</v>
       </c>
     </row>
     <row r="86">
@@ -2146,19 +2403,22 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>12.153358</v>
+        <v>10.44676</v>
       </c>
       <c r="C86" t="n">
-        <v>-0.0002536773681640625</v>
+        <v>1025.332763671875</v>
       </c>
       <c r="D86" t="n">
-        <v>148.2027282714844</v>
+        <v>7.609691143035889</v>
       </c>
       <c r="E86" t="n">
-        <v>29.0933952331543</v>
+        <v>14.56517505645752</v>
       </c>
       <c r="F86" t="n">
-        <v>9.981512448575813e-06</v>
+        <v>-0.8024211525917053</v>
+      </c>
+      <c r="G86" t="n">
+        <v>-3.154694080352783</v>
       </c>
     </row>
     <row r="87">
@@ -2166,19 +2426,22 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>12.321836</v>
+        <v>10.574801</v>
       </c>
       <c r="C87" t="n">
-        <v>-0.0002431869506835938</v>
+        <v>1025.332763671875</v>
       </c>
       <c r="D87" t="n">
-        <v>154.0687561035156</v>
+        <v>7.609691143035889</v>
       </c>
       <c r="E87" t="n">
-        <v>29.52888870239258</v>
+        <v>14.56517505645752</v>
       </c>
       <c r="F87" t="n">
-        <v>0.0001187699745059945</v>
+        <v>-0.8024211525917053</v>
+      </c>
+      <c r="G87" t="n">
+        <v>-3.154694080352783</v>
       </c>
     </row>
     <row r="88">
@@ -2186,19 +2449,22 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>12.475164</v>
+        <v>10.712576</v>
       </c>
       <c r="C88" t="n">
-        <v>-0.0002298355102539062</v>
+        <v>1026.80859375</v>
       </c>
       <c r="D88" t="n">
-        <v>157.0342864990234</v>
+        <v>7.528464794158936</v>
       </c>
       <c r="E88" t="n">
-        <v>29.7446117401123</v>
+        <v>14.89524173736572</v>
       </c>
       <c r="F88" t="n">
-        <v>0.0001597225054865703</v>
+        <v>-0.8195913434028625</v>
+      </c>
+      <c r="G88" t="n">
+        <v>-3.151184558868408</v>
       </c>
     </row>
     <row r="89">
@@ -2206,19 +2472,22 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>12.626158</v>
+        <v>10.848416</v>
       </c>
       <c r="C89" t="n">
-        <v>-0.0001916885375976562</v>
+        <v>1028.317138671875</v>
       </c>
       <c r="D89" t="n">
-        <v>163.0296783447266</v>
+        <v>7.445528507232666</v>
       </c>
       <c r="E89" t="n">
-        <v>30.17201614379883</v>
+        <v>15.22134208679199</v>
       </c>
       <c r="F89" t="n">
-        <v>0.0002340166829526424</v>
+        <v>-0.8361294865608215</v>
+      </c>
+      <c r="G89" t="n">
+        <v>-3.145905017852783</v>
       </c>
     </row>
     <row r="90">
@@ -2226,19 +2495,22 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>12.795181</v>
+        <v>10.98849</v>
       </c>
       <c r="C90" t="n">
-        <v>-0.0001659393310546875</v>
+        <v>1029.858154296875</v>
       </c>
       <c r="D90" t="n">
-        <v>166.0593109130859</v>
+        <v>7.360946655273438</v>
       </c>
       <c r="E90" t="n">
-        <v>30.38372230529785</v>
+        <v>15.54352378845215</v>
       </c>
       <c r="F90" t="n">
-        <v>0.0002594219404272735</v>
+        <v>-0.8521557450294495</v>
+      </c>
+      <c r="G90" t="n">
+        <v>-3.139465808868408</v>
       </c>
     </row>
     <row r="91">
@@ -2246,19 +2518,22 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>12.973479</v>
+        <v>11.120993</v>
       </c>
       <c r="C91" t="n">
-        <v>-0.000110626220703125</v>
+        <v>1029.858154296875</v>
       </c>
       <c r="D91" t="n">
-        <v>172.180419921875</v>
+        <v>7.360946655273438</v>
       </c>
       <c r="E91" t="n">
-        <v>30.77071762084961</v>
+        <v>15.54352378845215</v>
       </c>
       <c r="F91" t="n">
-        <v>0.0002877413935493678</v>
+        <v>-0.8521557450294495</v>
+      </c>
+      <c r="G91" t="n">
+        <v>-3.139465808868408</v>
       </c>
     </row>
     <row r="92">
@@ -2266,19 +2541,22 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>13.132423</v>
+        <v>11.262258</v>
       </c>
       <c r="C92" t="n">
-        <v>-8.106231689453125e-05</v>
+        <v>1031.431030273438</v>
       </c>
       <c r="D92" t="n">
-        <v>175.262939453125</v>
+        <v>7.274770736694336</v>
       </c>
       <c r="E92" t="n">
-        <v>30.85689926147461</v>
+        <v>15.86182308197021</v>
       </c>
       <c r="F92" t="n">
-        <v>0.0002897887607105076</v>
+        <v>-0.8677734136581421</v>
+      </c>
+      <c r="G92" t="n">
+        <v>-3.132477521896362</v>
       </c>
     </row>
     <row r="93">
@@ -2286,19 +2564,22 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>13.301998</v>
+        <v>11.401234</v>
       </c>
       <c r="C93" t="n">
-        <v>-5.245208740234375e-05</v>
+        <v>1033.033203125</v>
       </c>
       <c r="D93" t="n">
-        <v>178.3489532470703</v>
+        <v>7.169400691986084</v>
       </c>
       <c r="E93" t="n">
-        <v>30.86229515075684</v>
+        <v>16.1416015625</v>
       </c>
       <c r="F93" t="n">
-        <v>0.0002856638166122139</v>
+        <v>-1.196021676063538</v>
+      </c>
+      <c r="G93" t="n">
+        <v>-3.618103742599487</v>
       </c>
     </row>
     <row r="94">
@@ -2306,19 +2587,22 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>13.452732</v>
+        <v>11.540941</v>
       </c>
       <c r="C94" t="n">
-        <v>2.86102294921875e-06</v>
+        <v>1034.664428710938</v>
       </c>
       <c r="D94" t="n">
-        <v>184.5040588378906</v>
+        <v>7.040660381317139</v>
       </c>
       <c r="E94" t="n">
-        <v>30.68336296081543</v>
+        <v>16.4223461151123</v>
       </c>
       <c r="F94" t="n">
-        <v>0.0002599376603029668</v>
+        <v>-1.480881929397583</v>
+      </c>
+      <c r="G94" t="n">
+        <v>-4.620943069458008</v>
       </c>
     </row>
     <row r="95">
@@ -2326,19 +2610,22 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>13.641538</v>
+        <v>11.683867</v>
       </c>
       <c r="C95" t="n">
-        <v>5.054473876953125e-05</v>
+        <v>1034.664428710938</v>
       </c>
       <c r="D95" t="n">
-        <v>190.6041412353516</v>
+        <v>7.040660381317139</v>
       </c>
       <c r="E95" t="n">
-        <v>30.33957290649414</v>
+        <v>16.4223461151123</v>
       </c>
       <c r="F95" t="n">
-        <v>0.0002182952594012022</v>
+        <v>-1.480881929397583</v>
+      </c>
+      <c r="G95" t="n">
+        <v>-4.620943069458008</v>
       </c>
     </row>
     <row r="96">
@@ -2346,19 +2633,22 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>13.789632</v>
+        <v>11.81996</v>
       </c>
       <c r="C96" t="n">
-        <v>7.152557373046875e-05</v>
+        <v>1036.322998046875</v>
       </c>
       <c r="D96" t="n">
-        <v>193.62548828125</v>
+        <v>6.883400917053223</v>
       </c>
       <c r="E96" t="n">
-        <v>30.12950325012207</v>
+        <v>16.68780517578125</v>
       </c>
       <c r="F96" t="n">
-        <v>0.000193011830560863</v>
+        <v>-1.823136448860168</v>
+      </c>
+      <c r="G96" t="n">
+        <v>-5.888797283172607</v>
       </c>
     </row>
     <row r="97">
@@ -2366,19 +2656,22 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>13.986586</v>
+        <v>11.967655</v>
       </c>
       <c r="C97" t="n">
-        <v>0.0001058578491210938</v>
+        <v>1038.007690429688</v>
       </c>
       <c r="D97" t="n">
-        <v>199.6009063720703</v>
+        <v>6.69122838973999</v>
       </c>
       <c r="E97" t="n">
-        <v>29.66285514831543</v>
+        <v>16.93797874450684</v>
       </c>
       <c r="F97" t="n">
-        <v>0.0001337353169219568</v>
+        <v>-2.204539775848389</v>
+      </c>
+      <c r="G97" t="n">
+        <v>-7.273780345916748</v>
       </c>
     </row>
     <row r="98">
@@ -2386,19 +2679,22 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>14.1668</v>
+        <v>12.107994</v>
       </c>
       <c r="C98" t="n">
-        <v>0.0001173019409179688</v>
+        <v>1039.716796875</v>
       </c>
       <c r="D98" t="n">
-        <v>202.5525512695312</v>
+        <v>6.460826396942139</v>
       </c>
       <c r="E98" t="n">
-        <v>29.41444969177246</v>
+        <v>17.17680740356445</v>
       </c>
       <c r="F98" t="n">
-        <v>0.0001046038596541621</v>
+        <v>-2.596282958984375</v>
+      </c>
+      <c r="G98" t="n">
+        <v>-8.651379585266113</v>
       </c>
     </row>
     <row r="99">
@@ -2406,19 +2702,22 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>14.350736</v>
+        <v>12.256611</v>
       </c>
       <c r="C99" t="n">
-        <v>0.0001325607299804688</v>
+        <v>1041.449829101562</v>
       </c>
       <c r="D99" t="n">
-        <v>208.3808746337891</v>
+        <v>6.191465377807617</v>
       </c>
       <c r="E99" t="n">
-        <v>28.9289722442627</v>
+        <v>17.40855407714844</v>
       </c>
       <c r="F99" t="n">
-        <v>4.38441893493291e-05</v>
+        <v>-2.977402925491333</v>
+      </c>
+      <c r="G99" t="n">
+        <v>-9.92121696472168</v>
       </c>
     </row>
     <row r="100">
@@ -2426,19 +2725,22 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>14.509549</v>
+        <v>12.402076</v>
       </c>
       <c r="C100" t="n">
-        <v>0.0001363754272460938</v>
+        <v>1041.449829101562</v>
       </c>
       <c r="D100" t="n">
-        <v>211.2648162841797</v>
+        <v>6.191465377807617</v>
       </c>
       <c r="E100" t="n">
-        <v>28.78257179260254</v>
+        <v>17.40855407714844</v>
       </c>
       <c r="F100" t="n">
-        <v>1.494991101935739e-05</v>
+        <v>-2.977402925491333</v>
+      </c>
+      <c r="G100" t="n">
+        <v>-9.92121696472168</v>
       </c>
     </row>
     <row r="101">
@@ -2446,19 +2748,22 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>14.685465</v>
+        <v>12.543547</v>
       </c>
       <c r="C101" t="n">
-        <v>0.0001344680786132812</v>
+        <v>1043.205932617188</v>
       </c>
       <c r="D101" t="n">
-        <v>217.0094909667969</v>
+        <v>5.88463830947876</v>
       </c>
       <c r="E101" t="n">
-        <v>28.69833755493164</v>
+        <v>17.63856506347656</v>
       </c>
       <c r="F101" t="n">
-        <v>-3.751344775082543e-05</v>
+        <v>-3.328850269317627</v>
+      </c>
+      <c r="G101" t="n">
+        <v>-11.01155090332031</v>
       </c>
     </row>
     <row r="102">
@@ -2466,19 +2771,22 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>14.868563</v>
+        <v>12.697435</v>
       </c>
       <c r="C102" t="n">
-        <v>0.00012969970703125</v>
+        <v>1044.985229492188</v>
       </c>
       <c r="D102" t="n">
-        <v>219.8816680908203</v>
+        <v>5.543717384338379</v>
       </c>
       <c r="E102" t="n">
-        <v>28.73180770874023</v>
+        <v>17.8721752166748</v>
       </c>
       <c r="F102" t="n">
-        <v>-5.967025208519772e-05</v>
+        <v>-3.635523080825806</v>
+      </c>
+      <c r="G102" t="n">
+        <v>-11.8770923614502</v>
       </c>
     </row>
     <row r="103">
@@ -2486,19 +2794,22 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>15.037554</v>
+        <v>12.847524</v>
       </c>
       <c r="C103" t="n">
-        <v>0.00011444091796875</v>
+        <v>1046.7880859375</v>
       </c>
       <c r="D103" t="n">
-        <v>225.6454315185547</v>
+        <v>5.173484802246094</v>
       </c>
       <c r="E103" t="n">
-        <v>28.89664077758789</v>
+        <v>18.11360740661621</v>
       </c>
       <c r="F103" t="n">
-        <v>-9.798118844628334e-05</v>
+        <v>-3.887078762054443</v>
+      </c>
+      <c r="G103" t="n">
+        <v>-12.49666404724121</v>
       </c>
     </row>
     <row r="104">
@@ -2506,19 +2817,22 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>15.20893</v>
+        <v>12.9935</v>
       </c>
       <c r="C104" t="n">
-        <v>0.0001039505004882812</v>
+        <v>1048.615356445312</v>
       </c>
       <c r="D104" t="n">
-        <v>228.5423736572266</v>
+        <v>4.77963924407959</v>
       </c>
       <c r="E104" t="n">
-        <v>29.01438140869141</v>
+        <v>18.36545562744141</v>
       </c>
       <c r="F104" t="n">
-        <v>-0.0001146391950896941</v>
+        <v>-4.078084468841553</v>
+      </c>
+      <c r="G104" t="n">
+        <v>-12.86998462677002</v>
       </c>
     </row>
     <row r="105">
@@ -2526,19 +2840,22 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>15.386182</v>
+        <v>13.159071</v>
       </c>
       <c r="C105" t="n">
-        <v>7.82012939453125e-05</v>
+        <v>1050.468139648438</v>
       </c>
       <c r="D105" t="n">
-        <v>234.3759460449219</v>
+        <v>4.368278503417969</v>
       </c>
       <c r="E105" t="n">
-        <v>29.29769706726074</v>
+        <v>18.62851333618164</v>
       </c>
       <c r="F105" t="n">
-        <v>-0.0001450305280741304</v>
+        <v>-4.207977771759033</v>
+      </c>
+      <c r="G105" t="n">
+        <v>-13.01442337036133</v>
       </c>
     </row>
     <row r="106">
@@ -2546,19 +2863,22 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>15.562231</v>
+        <v>13.303309</v>
       </c>
       <c r="C106" t="n">
-        <v>4.9591064453125e-05</v>
+        <v>1050.468139648438</v>
       </c>
       <c r="D106" t="n">
-        <v>240.2710266113281</v>
+        <v>4.368278503417969</v>
       </c>
       <c r="E106" t="n">
-        <v>29.62492942810059</v>
+        <v>18.62851333618164</v>
       </c>
       <c r="F106" t="n">
-        <v>-0.0001561127428431064</v>
+        <v>-4.207977771759033</v>
+      </c>
+      <c r="G106" t="n">
+        <v>-13.01442337036133</v>
       </c>
     </row>
     <row r="107">
@@ -2566,19 +2886,22 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>15.712485</v>
+        <v>13.454582</v>
       </c>
       <c r="C107" t="n">
-        <v>3.528594970703125e-05</v>
+        <v>1052.347534179688</v>
       </c>
       <c r="D107" t="n">
-        <v>243.2439270019531</v>
+        <v>3.945422887802124</v>
       </c>
       <c r="E107" t="n">
-        <v>29.79974937438965</v>
+        <v>18.9019947052002</v>
       </c>
       <c r="F107" t="n">
-        <v>-0.000157805290655233</v>
+        <v>-4.280540466308594</v>
+      </c>
+      <c r="G107" t="n">
+        <v>-12.96074295043945</v>
       </c>
     </row>
     <row r="108">
@@ -2586,19 +2909,22 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>15.887378</v>
+        <v>13.609555</v>
       </c>
       <c r="C108" t="n">
-        <v>2.09808349609375e-05</v>
+        <v>1054.25439453125</v>
       </c>
       <c r="D108" t="n">
-        <v>246.2345886230469</v>
+        <v>3.516614675521851</v>
       </c>
       <c r="E108" t="n">
-        <v>29.98002433776855</v>
+        <v>19.18403434753418</v>
       </c>
       <c r="F108" t="n">
-        <v>-0.0001560210657771677</v>
+        <v>-4.302825450897217</v>
+      </c>
+      <c r="G108" t="n">
+        <v>-12.74827861785889</v>
       </c>
     </row>
     <row r="109">
@@ -2606,19 +2932,22 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>16.080091</v>
+        <v>13.757345</v>
       </c>
       <c r="C109" t="n">
-        <v>-9.5367431640625e-06</v>
+        <v>1056.189575195312</v>
       </c>
       <c r="D109" t="n">
-        <v>252.2710876464844</v>
+        <v>3.086619138717651</v>
       </c>
       <c r="E109" t="n">
-        <v>30.3525447845459</v>
+        <v>19.47221183776855</v>
       </c>
       <c r="F109" t="n">
-        <v>-0.0001410512340953574</v>
+        <v>-4.284116268157959</v>
+      </c>
+      <c r="G109" t="n">
+        <v>-12.42030811309814</v>
       </c>
     </row>
     <row r="110">
@@ -2626,19 +2955,22 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>16.269112</v>
+        <v>13.910675</v>
       </c>
       <c r="C110" t="n">
-        <v>-3.528594970703125e-05</v>
+        <v>1058.153442382812</v>
       </c>
       <c r="D110" t="n">
-        <v>258.371826171875</v>
+        <v>2.65923547744751</v>
       </c>
       <c r="E110" t="n">
-        <v>30.57968902587891</v>
+        <v>19.76395797729492</v>
       </c>
       <c r="F110" t="n">
-        <v>-0.0001151477990788408</v>
+        <v>-4.234859943389893</v>
+      </c>
+      <c r="G110" t="n">
+        <v>-12.02000713348389</v>
       </c>
     </row>
     <row r="111">
@@ -2646,19 +2978,22 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>16.43675</v>
+        <v>14.066612</v>
       </c>
       <c r="C111" t="n">
-        <v>-4.673004150390625e-05</v>
+        <v>1060.146362304688</v>
       </c>
       <c r="D111" t="n">
-        <v>261.4293823242188</v>
+        <v>2.23720908164978</v>
       </c>
       <c r="E111" t="n">
-        <v>30.57136344909668</v>
+        <v>20.05688858032227</v>
       </c>
       <c r="F111" t="n">
-        <v>-9.918106661643833e-05</v>
+        <v>-4.165743827819824</v>
+      </c>
+      <c r="G111" t="n">
+        <v>-11.58720684051514</v>
       </c>
     </row>
     <row r="112">
@@ -2666,19 +3001,22 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>16.6125</v>
+        <v>14.216192</v>
       </c>
       <c r="C112" t="n">
-        <v>-6.29425048828125e-05</v>
+        <v>1060.146362304688</v>
       </c>
       <c r="D112" t="n">
-        <v>267.5242614746094</v>
+        <v>2.23720908164978</v>
       </c>
       <c r="E112" t="n">
-        <v>30.37475776672363</v>
+        <v>20.05688858032227</v>
       </c>
       <c r="F112" t="n">
-        <v>-6.381511775543913e-05</v>
+        <v>-4.165743827819824</v>
+      </c>
+      <c r="G112" t="n">
+        <v>-11.58720684051514</v>
       </c>
     </row>
     <row r="113">
@@ -2686,19 +3024,22 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>16.787057</v>
+        <v>14.371805</v>
       </c>
       <c r="C113" t="n">
-        <v>-6.771087646484375e-05</v>
+        <v>1062.168579101562</v>
       </c>
       <c r="D113" t="n">
-        <v>270.5519409179688</v>
+        <v>1.822231531143188</v>
       </c>
       <c r="E113" t="n">
-        <v>30.21350479125977</v>
+        <v>20.34895706176758</v>
       </c>
       <c r="F113" t="n">
-        <v>-4.488359627430327e-05</v>
+        <v>-4.08696174621582</v>
+      </c>
+      <c r="G113" t="n">
+        <v>-11.15645027160645</v>
       </c>
     </row>
     <row r="114">
@@ -2706,19 +3047,22 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>16.980826</v>
+        <v>14.537006</v>
       </c>
       <c r="C114" t="n">
-        <v>-7.343292236328125e-05</v>
+        <v>1064.219604492188</v>
       </c>
       <c r="D114" t="n">
-        <v>276.5515441894531</v>
+        <v>1.41500449180603</v>
       </c>
       <c r="E114" t="n">
-        <v>29.81265640258789</v>
+        <v>20.6385498046875</v>
       </c>
       <c r="F114" t="n">
-        <v>-5.028127816331107e-06</v>
+        <v>-4.007652759552002</v>
+      </c>
+      <c r="G114" t="n">
+        <v>-10.75553894042969</v>
       </c>
     </row>
     <row r="115">
@@ -2726,19 +3070,1287 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>17.162576</v>
+        <v>14.69738</v>
       </c>
       <c r="C115" t="n">
-        <v>-7.43865966796875e-05</v>
+        <v>1066.299560546875</v>
       </c>
       <c r="D115" t="n">
-        <v>279.519287109375</v>
+        <v>1.01535701751709</v>
       </c>
       <c r="E115" t="n">
-        <v>29.58577537536621</v>
+        <v>20.92446327209473</v>
       </c>
       <c r="F115" t="n">
-        <v>1.132633497036295e-05</v>
+        <v>-3.935525178909302</v>
+      </c>
+      <c r="G115" t="n">
+        <v>-10.40498352050781</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" t="n">
+        <v>14.849813</v>
+      </c>
+      <c r="C116" t="n">
+        <v>1068.407958984375</v>
+      </c>
+      <c r="D116" t="n">
+        <v>0.6223960518836975</v>
+      </c>
+      <c r="E116" t="n">
+        <v>21.20586776733398</v>
+      </c>
+      <c r="F116" t="n">
+        <v>-3.876605749130249</v>
+      </c>
+      <c r="G116" t="n">
+        <v>-10.11802673339844</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" t="n">
+        <v>15.008888</v>
+      </c>
+      <c r="C117" t="n">
+        <v>1070.544311523438</v>
+      </c>
+      <c r="D117" t="n">
+        <v>0.2346799373626709</v>
+      </c>
+      <c r="E117" t="n">
+        <v>21.48226547241211</v>
+      </c>
+      <c r="F117" t="n">
+        <v>-3.83514142036438</v>
+      </c>
+      <c r="G117" t="n">
+        <v>-9.90131950378418</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B118" t="n">
+        <v>15.174469</v>
+      </c>
+      <c r="C118" t="n">
+        <v>1072.7080078125</v>
+      </c>
+      <c r="D118" t="n">
+        <v>-0.149606466293335</v>
+      </c>
+      <c r="E118" t="n">
+        <v>21.75338554382324</v>
+      </c>
+      <c r="F118" t="n">
+        <v>-3.81367015838623</v>
+      </c>
+      <c r="G118" t="n">
+        <v>-9.755661010742188</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="B119" t="n">
+        <v>15.332422</v>
+      </c>
+      <c r="C119" t="n">
+        <v>1072.7080078125</v>
+      </c>
+      <c r="D119" t="n">
+        <v>-0.149606466293335</v>
+      </c>
+      <c r="E119" t="n">
+        <v>21.75338554382324</v>
+      </c>
+      <c r="F119" t="n">
+        <v>-3.81367015838623</v>
+      </c>
+      <c r="G119" t="n">
+        <v>-9.755661010742188</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="B120" t="n">
+        <v>15.485119</v>
+      </c>
+      <c r="C120" t="n">
+        <v>1074.898681640625</v>
+      </c>
+      <c r="D120" t="n">
+        <v>-0.5324850082397461</v>
+      </c>
+      <c r="E120" t="n">
+        <v>22.01918411254883</v>
+      </c>
+      <c r="F120" t="n">
+        <v>-3.813204526901245</v>
+      </c>
+      <c r="G120" t="n">
+        <v>-9.67744255065918</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B121" t="n">
+        <v>15.642773</v>
+      </c>
+      <c r="C121" t="n">
+        <v>1077.110107421875</v>
+      </c>
+      <c r="D121" t="n">
+        <v>-0.9386793971061707</v>
+      </c>
+      <c r="E121" t="n">
+        <v>22.17850494384766</v>
+      </c>
+      <c r="F121" t="n">
+        <v>-4.252508163452148</v>
+      </c>
+      <c r="G121" t="n">
+        <v>-10.28917026519775</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" t="n">
+        <v>15.804329</v>
+      </c>
+      <c r="C122" t="n">
+        <v>1079.33837890625</v>
+      </c>
+      <c r="D122" t="n">
+        <v>-1.381850361824036</v>
+      </c>
+      <c r="E122" t="n">
+        <v>22.32456016540527</v>
+      </c>
+      <c r="F122" t="n">
+        <v>-4.724204063415527</v>
+      </c>
+      <c r="G122" t="n">
+        <v>-11.75468921661377</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B123" t="n">
+        <v>15.966521</v>
+      </c>
+      <c r="C123" t="n">
+        <v>1081.570434570312</v>
+      </c>
+      <c r="D123" t="n">
+        <v>-1.893348336219788</v>
+      </c>
+      <c r="E123" t="n">
+        <v>22.25547981262207</v>
+      </c>
+      <c r="F123" t="n">
+        <v>-5.687849998474121</v>
+      </c>
+      <c r="G123" t="n">
+        <v>-14.30571460723877</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" t="n">
+        <v>16.145751</v>
+      </c>
+      <c r="C124" t="n">
+        <v>1083.804931640625</v>
+      </c>
+      <c r="D124" t="n">
+        <v>-2.477503061294556</v>
+      </c>
+      <c r="E124" t="n">
+        <v>22.29160118103027</v>
+      </c>
+      <c r="F124" t="n">
+        <v>-6.397495746612549</v>
+      </c>
+      <c r="G124" t="n">
+        <v>-17.30768966674805</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" t="n">
+        <v>16.304133</v>
+      </c>
+      <c r="C125" t="n">
+        <v>1086.037719726562</v>
+      </c>
+      <c r="D125" t="n">
+        <v>-3.144207000732422</v>
+      </c>
+      <c r="E125" t="n">
+        <v>22.22880744934082</v>
+      </c>
+      <c r="F125" t="n">
+        <v>-7.273129940032959</v>
+      </c>
+      <c r="G125" t="n">
+        <v>-20.14031791687012</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" t="n">
+        <v>16.464008</v>
+      </c>
+      <c r="C126" t="n">
+        <v>1088.261962890625</v>
+      </c>
+      <c r="D126" t="n">
+        <v>-3.90177321434021</v>
+      </c>
+      <c r="E126" t="n">
+        <v>22.12738037109375</v>
+      </c>
+      <c r="F126" t="n">
+        <v>-8.162338256835938</v>
+      </c>
+      <c r="G126" t="n">
+        <v>-22.68739318847656</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="B127" t="n">
+        <v>16.630113</v>
+      </c>
+      <c r="C127" t="n">
+        <v>1090.475708007812</v>
+      </c>
+      <c r="D127" t="n">
+        <v>-4.748083591461182</v>
+      </c>
+      <c r="E127" t="n">
+        <v>22.02480888366699</v>
+      </c>
+      <c r="F127" t="n">
+        <v>-8.99769401550293</v>
+      </c>
+      <c r="G127" t="n">
+        <v>-24.80402565002441</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" t="n">
+        <v>16.802597</v>
+      </c>
+      <c r="C128" t="n">
+        <v>1092.679931640625</v>
+      </c>
+      <c r="D128" t="n">
+        <v>-5.675973415374756</v>
+      </c>
+      <c r="E128" t="n">
+        <v>21.95111274719238</v>
+      </c>
+      <c r="F128" t="n">
+        <v>-9.737455368041992</v>
+      </c>
+      <c r="G128" t="n">
+        <v>-26.37956047058105</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" t="n">
+        <v>16.971905</v>
+      </c>
+      <c r="C129" t="n">
+        <v>1094.879150390625</v>
+      </c>
+      <c r="D129" t="n">
+        <v>-6.67384147644043</v>
+      </c>
+      <c r="E129" t="n">
+        <v>21.93803596496582</v>
+      </c>
+      <c r="F129" t="n">
+        <v>-10.33987998962402</v>
+      </c>
+      <c r="G129" t="n">
+        <v>-27.34886360168457</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" t="n">
+        <v>17.148574</v>
+      </c>
+      <c r="C130" t="n">
+        <v>1097.08056640625</v>
+      </c>
+      <c r="D130" t="n">
+        <v>-7.726149082183838</v>
+      </c>
+      <c r="E130" t="n">
+        <v>22.01033401489258</v>
+      </c>
+      <c r="F130" t="n">
+        <v>-10.77165412902832</v>
+      </c>
+      <c r="G130" t="n">
+        <v>-27.69169998168945</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" t="n">
+        <v>17.328642</v>
+      </c>
+      <c r="C131" t="n">
+        <v>1099.293212890625</v>
+      </c>
+      <c r="D131" t="n">
+        <v>-8.814452171325684</v>
+      </c>
+      <c r="E131" t="n">
+        <v>22.18011093139648</v>
+      </c>
+      <c r="F131" t="n">
+        <v>-11.01162719726562</v>
+      </c>
+      <c r="G131" t="n">
+        <v>-27.43647575378418</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" t="n">
+        <v>17.490156</v>
+      </c>
+      <c r="C132" t="n">
+        <v>1099.293212890625</v>
+      </c>
+      <c r="D132" t="n">
+        <v>-8.814452171325684</v>
+      </c>
+      <c r="E132" t="n">
+        <v>22.18011093139648</v>
+      </c>
+      <c r="F132" t="n">
+        <v>-11.01162719726562</v>
+      </c>
+      <c r="G132" t="n">
+        <v>-27.43647575378418</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" t="n">
+        <v>17.65361</v>
+      </c>
+      <c r="C133" t="n">
+        <v>1101.526733398438</v>
+      </c>
+      <c r="D133" t="n">
+        <v>-9.919038772583008</v>
+      </c>
+      <c r="E133" t="n">
+        <v>22.44217300415039</v>
+      </c>
+      <c r="F133" t="n">
+        <v>-11.05768394470215</v>
+      </c>
+      <c r="G133" t="n">
+        <v>-26.6612377166748</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" t="n">
+        <v>17.820798</v>
+      </c>
+      <c r="C134" t="n">
+        <v>1103.789306640625</v>
+      </c>
+      <c r="D134" t="n">
+        <v>-11.02103328704834</v>
+      </c>
+      <c r="E134" t="n">
+        <v>22.77850723266602</v>
+      </c>
+      <c r="F134" t="n">
+        <v>-10.92797565460205</v>
+      </c>
+      <c r="G134" t="n">
+        <v>-25.48313522338867</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" t="n">
+        <v>17.984857</v>
+      </c>
+      <c r="C135" t="n">
+        <v>1106.08740234375</v>
+      </c>
+      <c r="D135" t="n">
+        <v>-12.10405254364014</v>
+      </c>
+      <c r="E135" t="n">
+        <v>23.16633987426758</v>
+      </c>
+      <c r="F135" t="n">
+        <v>-10.65233039855957</v>
+      </c>
+      <c r="G135" t="n">
+        <v>-24.03153228759766</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" t="n">
+        <v>18.157853</v>
+      </c>
+      <c r="C136" t="n">
+        <v>1108.424926757812</v>
+      </c>
+      <c r="D136" t="n">
+        <v>-13.15494823455811</v>
+      </c>
+      <c r="E136" t="n">
+        <v>23.58420372009277</v>
+      </c>
+      <c r="F136" t="n">
+        <v>-10.26431655883789</v>
+      </c>
+      <c r="G136" t="n">
+        <v>-22.42597770690918</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" t="n">
+        <v>18.330082</v>
+      </c>
+      <c r="C137" t="n">
+        <v>1110.804321289062</v>
+      </c>
+      <c r="D137" t="n">
+        <v>-14.16383647918701</v>
+      </c>
+      <c r="E137" t="n">
+        <v>24.0147819519043</v>
+      </c>
+      <c r="F137" t="n">
+        <v>-9.795738220214844</v>
+      </c>
+      <c r="G137" t="n">
+        <v>-20.76641273498535</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" t="n">
+        <v>18.502122</v>
+      </c>
+      <c r="C138" t="n">
+        <v>1113.226684570312</v>
+      </c>
+      <c r="D138" t="n">
+        <v>-15.12377643585205</v>
+      </c>
+      <c r="E138" t="n">
+        <v>24.44549751281738</v>
+      </c>
+      <c r="F138" t="n">
+        <v>-9.273978233337402</v>
+      </c>
+      <c r="G138" t="n">
+        <v>-19.12789916992188</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" t="n">
+        <v>18.676575</v>
+      </c>
+      <c r="C139" t="n">
+        <v>1115.683837890625</v>
+      </c>
+      <c r="D139" t="n">
+        <v>-16.05650520324707</v>
+      </c>
+      <c r="E139" t="n">
+        <v>24.72602653503418</v>
+      </c>
+      <c r="F139" t="n">
+        <v>-9.197158813476562</v>
+      </c>
+      <c r="G139" t="n">
+        <v>-18.29483985900879</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" t="n">
+        <v>18.846906</v>
+      </c>
+      <c r="C140" t="n">
+        <v>1118.171020507812</v>
+      </c>
+      <c r="D140" t="n">
+        <v>-16.9763298034668</v>
+      </c>
+      <c r="E140" t="n">
+        <v>24.97701454162598</v>
+      </c>
+      <c r="F140" t="n">
+        <v>-9.19938850402832</v>
+      </c>
+      <c r="G140" t="n">
+        <v>-18.58264541625977</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" t="n">
+        <v>19.017613</v>
+      </c>
+      <c r="C141" t="n">
+        <v>1120.680786132812</v>
+      </c>
+      <c r="D141" t="n">
+        <v>-17.90362358093262</v>
+      </c>
+      <c r="E141" t="n">
+        <v>25.12981414794922</v>
+      </c>
+      <c r="F141" t="n">
+        <v>-9.452360153198242</v>
+      </c>
+      <c r="G141" t="n">
+        <v>-19.81091117858887</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" t="n">
+        <v>19.189547</v>
+      </c>
+      <c r="C142" t="n">
+        <v>1123.189086914062</v>
+      </c>
+      <c r="D142" t="n">
+        <v>-18.88469886779785</v>
+      </c>
+      <c r="E142" t="n">
+        <v>24.94273376464844</v>
+      </c>
+      <c r="F142" t="n">
+        <v>-10.31371212005615</v>
+      </c>
+      <c r="G142" t="n">
+        <v>-22.34892272949219</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" t="n">
+        <v>19.358963</v>
+      </c>
+      <c r="C143" t="n">
+        <v>1125.674438476562</v>
+      </c>
+      <c r="D143" t="n">
+        <v>-19.95333862304688</v>
+      </c>
+      <c r="E143" t="n">
+        <v>24.60149192810059</v>
+      </c>
+      <c r="F143" t="n">
+        <v>-11.36314582824707</v>
+      </c>
+      <c r="G143" t="n">
+        <v>-26.15690040588379</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" t="n">
+        <v>19.534579</v>
+      </c>
+      <c r="C144" t="n">
+        <v>1128.133056640625</v>
+      </c>
+      <c r="D144" t="n">
+        <v>-21.11541938781738</v>
+      </c>
+      <c r="E144" t="n">
+        <v>24.31740760803223</v>
+      </c>
+      <c r="F144" t="n">
+        <v>-12.30807018280029</v>
+      </c>
+      <c r="G144" t="n">
+        <v>-30.11728286743164</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" t="n">
+        <v>19.714987</v>
+      </c>
+      <c r="C145" t="n">
+        <v>1130.552490234375</v>
+      </c>
+      <c r="D145" t="n">
+        <v>-22.3847599029541</v>
+      </c>
+      <c r="E145" t="n">
+        <v>23.86689376831055</v>
+      </c>
+      <c r="F145" t="n">
+        <v>-13.40026950836182</v>
+      </c>
+      <c r="G145" t="n">
+        <v>-33.66481399536133</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" t="n">
+        <v>19.894074</v>
+      </c>
+      <c r="C146" t="n">
+        <v>1132.92236328125</v>
+      </c>
+      <c r="D146" t="n">
+        <v>-23.76697731018066</v>
+      </c>
+      <c r="E146" t="n">
+        <v>23.36271858215332</v>
+      </c>
+      <c r="F146" t="n">
+        <v>-14.48318481445312</v>
+      </c>
+      <c r="G146" t="n">
+        <v>-36.67113494873047</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B147" t="n">
+        <v>20.074744</v>
+      </c>
+      <c r="C147" t="n">
+        <v>1135.240478515625</v>
+      </c>
+      <c r="D147" t="n">
+        <v>-25.2575626373291</v>
+      </c>
+      <c r="E147" t="n">
+        <v>22.8715763092041</v>
+      </c>
+      <c r="F147" t="n">
+        <v>-15.4919605255127</v>
+      </c>
+      <c r="G147" t="n">
+        <v>-38.98728561401367</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B148" t="n">
+        <v>20.260701</v>
+      </c>
+      <c r="C148" t="n">
+        <v>1137.511352539062</v>
+      </c>
+      <c r="D148" t="n">
+        <v>-26.84662246704102</v>
+      </c>
+      <c r="E148" t="n">
+        <v>22.45623779296875</v>
+      </c>
+      <c r="F148" t="n">
+        <v>-16.3766040802002</v>
+      </c>
+      <c r="G148" t="n">
+        <v>-40.49435043334961</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B149" t="n">
+        <v>20.444484</v>
+      </c>
+      <c r="C149" t="n">
+        <v>1139.74609375</v>
+      </c>
+      <c r="D149" t="n">
+        <v>-28.5188102722168</v>
+      </c>
+      <c r="E149" t="n">
+        <v>22.18506622314453</v>
+      </c>
+      <c r="F149" t="n">
+        <v>-17.08134269714355</v>
+      </c>
+      <c r="G149" t="n">
+        <v>-41.11169815063477</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B150" t="n">
+        <v>20.625097</v>
+      </c>
+      <c r="C150" t="n">
+        <v>1141.962524414062</v>
+      </c>
+      <c r="D150" t="n">
+        <v>-30.25265502929688</v>
+      </c>
+      <c r="E150" t="n">
+        <v>22.12061500549316</v>
+      </c>
+      <c r="F150" t="n">
+        <v>-17.54599761962891</v>
+      </c>
+      <c r="G150" t="n">
+        <v>-40.80755615234375</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B151" t="n">
+        <v>20.806123</v>
+      </c>
+      <c r="C151" t="n">
+        <v>1144.183471679688</v>
+      </c>
+      <c r="D151" t="n">
+        <v>-32.02064514160156</v>
+      </c>
+      <c r="E151" t="n">
+        <v>22.29623985290527</v>
+      </c>
+      <c r="F151" t="n">
+        <v>-17.71809005737305</v>
+      </c>
+      <c r="G151" t="n">
+        <v>-39.62181091308594</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B152" t="n">
+        <v>20.987433</v>
+      </c>
+      <c r="C152" t="n">
+        <v>1146.43212890625</v>
+      </c>
+      <c r="D152" t="n">
+        <v>-33.79189300537109</v>
+      </c>
+      <c r="E152" t="n">
+        <v>22.6906681060791</v>
+      </c>
+      <c r="F152" t="n">
+        <v>-17.58538818359375</v>
+      </c>
+      <c r="G152" t="n">
+        <v>-37.69709396362305</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="B153" t="n">
+        <v>21.173478</v>
+      </c>
+      <c r="C153" t="n">
+        <v>1148.735961914062</v>
+      </c>
+      <c r="D153" t="n">
+        <v>-35.51735687255859</v>
+      </c>
+      <c r="E153" t="n">
+        <v>23.40810203552246</v>
+      </c>
+      <c r="F153" t="n">
+        <v>-16.81055068969727</v>
+      </c>
+      <c r="G153" t="n">
+        <v>-34.68760681152344</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B154" t="n">
+        <v>21.352972</v>
+      </c>
+      <c r="C154" t="n">
+        <v>1151.109497070312</v>
+      </c>
+      <c r="D154" t="n">
+        <v>-37.15871429443359</v>
+      </c>
+      <c r="E154" t="n">
+        <v>24.18505096435547</v>
+      </c>
+      <c r="F154" t="n">
+        <v>-15.77460765838623</v>
+      </c>
+      <c r="G154" t="n">
+        <v>-30.56226348876953</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="B155" t="n">
+        <v>21.534294</v>
+      </c>
+      <c r="C155" t="n">
+        <v>1153.547607421875</v>
+      </c>
+      <c r="D155" t="n">
+        <v>-38.72647857666016</v>
+      </c>
+      <c r="E155" t="n">
+        <v>24.77659606933594</v>
+      </c>
+      <c r="F155" t="n">
+        <v>-15.17171001434326</v>
+      </c>
+      <c r="G155" t="n">
+        <v>-26.80875778198242</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B156" t="n">
+        <v>21.715482</v>
+      </c>
+      <c r="C156" t="n">
+        <v>1156.052001953125</v>
+      </c>
+      <c r="D156" t="n">
+        <v>-40.21719360351562</v>
+      </c>
+      <c r="E156" t="n">
+        <v>25.39883804321289</v>
+      </c>
+      <c r="F156" t="n">
+        <v>-14.41794967651367</v>
+      </c>
+      <c r="G156" t="n">
+        <v>-24.33088111877441</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="B157" t="n">
+        <v>21.902787</v>
+      </c>
+      <c r="C157" t="n">
+        <v>1158.619506835938</v>
+      </c>
+      <c r="D157" t="n">
+        <v>-41.62984466552734</v>
+      </c>
+      <c r="E157" t="n">
+        <v>25.94420623779297</v>
+      </c>
+      <c r="F157" t="n">
+        <v>-13.79000186920166</v>
+      </c>
+      <c r="G157" t="n">
+        <v>-23.14402198791504</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="B158" t="n">
+        <v>22.085447</v>
+      </c>
+      <c r="C158" t="n">
+        <v>1161.2265625</v>
+      </c>
+      <c r="D158" t="n">
+        <v>-43.00911712646484</v>
+      </c>
+      <c r="E158" t="n">
+        <v>26.10647392272949</v>
+      </c>
+      <c r="F158" t="n">
+        <v>-13.88828086853027</v>
+      </c>
+      <c r="G158" t="n">
+        <v>-24.03001022338867</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="B159" t="n">
+        <v>22.273022</v>
+      </c>
+      <c r="C159" t="n">
+        <v>1163.839233398438</v>
+      </c>
+      <c r="D159" t="n">
+        <v>-44.41377639770508</v>
+      </c>
+      <c r="E159" t="n">
+        <v>25.92437744140625</v>
+      </c>
+      <c r="F159" t="n">
+        <v>-14.52184772491455</v>
+      </c>
+      <c r="G159" t="n">
+        <v>-27.53941535949707</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="B160" t="n">
+        <v>22.461753</v>
+      </c>
+      <c r="C160" t="n">
+        <v>1166.41796875</v>
+      </c>
+      <c r="D160" t="n">
+        <v>-45.89840316772461</v>
+      </c>
+      <c r="E160" t="n">
+        <v>25.31876945495605</v>
+      </c>
+      <c r="F160" t="n">
+        <v>-15.62912273406982</v>
+      </c>
+      <c r="G160" t="n">
+        <v>-32.97633361816406</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="B161" t="n">
+        <v>22.657083</v>
+      </c>
+      <c r="C161" t="n">
+        <v>1168.921020507812</v>
+      </c>
+      <c r="D161" t="n">
+        <v>-47.50206756591797</v>
+      </c>
+      <c r="E161" t="n">
+        <v>24.3514575958252</v>
+      </c>
+      <c r="F161" t="n">
+        <v>-16.95822334289551</v>
+      </c>
+      <c r="G161" t="n">
+        <v>-39.41172790527344</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="B162" t="n">
+        <v>22.852954</v>
+      </c>
+      <c r="C162" t="n">
+        <v>1171.317138671875</v>
+      </c>
+      <c r="D162" t="n">
+        <v>-49.23986053466797</v>
+      </c>
+      <c r="E162" t="n">
+        <v>23.14422988891602</v>
+      </c>
+      <c r="F162" t="n">
+        <v>-18.32054328918457</v>
+      </c>
+      <c r="G162" t="n">
+        <v>-46.06095504760742</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="B163" t="n">
+        <v>23.046324</v>
+      </c>
+      <c r="C163" t="n">
+        <v>1173.596801757812</v>
+      </c>
+      <c r="D163" t="n">
+        <v>-51.10866928100586</v>
+      </c>
+      <c r="E163" t="n">
+        <v>21.96867370605469</v>
+      </c>
+      <c r="F163" t="n">
+        <v>-19.5716495513916</v>
+      </c>
+      <c r="G163" t="n">
+        <v>-52.14787673950195</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="B164" t="n">
+        <v>23.235297</v>
+      </c>
+      <c r="C164" t="n">
+        <v>1175.7626953125</v>
+      </c>
+      <c r="D164" t="n">
+        <v>-53.08778762817383</v>
+      </c>
+      <c r="E164" t="n">
+        <v>20.81642723083496</v>
+      </c>
+      <c r="F164" t="n">
+        <v>-20.55011749267578</v>
+      </c>
+      <c r="G164" t="n">
+        <v>-57.16569519042969</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="B165" t="n">
+        <v>23.422438</v>
+      </c>
+      <c r="C165" t="n">
+        <v>1177.7900390625</v>
+      </c>
+      <c r="D165" t="n">
+        <v>-55.18049240112305</v>
+      </c>
+      <c r="E165" t="n">
+        <v>19.3598747253418</v>
+      </c>
+      <c r="F165" t="n">
+        <v>-21.69199752807617</v>
+      </c>
+      <c r="G165" t="n">
+        <v>-60.92809677124023</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="B166" t="n">
+        <v>23.626221</v>
+      </c>
+      <c r="C166" t="n">
+        <v>1179.68212890625</v>
+      </c>
+      <c r="D166" t="n">
+        <v>-57.38317108154297</v>
+      </c>
+      <c r="E166" t="n">
+        <v>18.11981391906738</v>
+      </c>
+      <c r="F166" t="n">
+        <v>-22.61265754699707</v>
+      </c>
+      <c r="G166" t="n">
+        <v>-63.53164291381836</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="n">
+        <v>165</v>
+      </c>
+      <c r="B167" t="n">
+        <v>23.820338</v>
+      </c>
+      <c r="C167" t="n">
+        <v>1183.152221679688</v>
+      </c>
+      <c r="D167" t="n">
+        <v>-62.06083297729492</v>
+      </c>
+      <c r="E167" t="n">
+        <v>17.00092315673828</v>
+      </c>
+      <c r="F167" t="n">
+        <v>-23.86683464050293</v>
+      </c>
+      <c r="G167" t="n">
+        <v>-62.19561767578125</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="n">
+        <v>166</v>
+      </c>
+      <c r="B168" t="n">
+        <v>24.012633</v>
+      </c>
+      <c r="C168" t="n">
+        <v>1184.8408203125</v>
+      </c>
+      <c r="D168" t="n">
+        <v>-64.48098754882812</v>
+      </c>
+      <c r="E168" t="n">
+        <v>17.31002426147461</v>
+      </c>
+      <c r="F168" t="n">
+        <v>-23.94106101989746</v>
+      </c>
+      <c r="G168" t="n">
+        <v>-57.40818786621094</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="B169" t="n">
+        <v>24.208915</v>
+      </c>
+      <c r="C169" t="n">
+        <v>1186.593994140625</v>
+      </c>
+      <c r="D169" t="n">
+        <v>-66.881591796875</v>
+      </c>
+      <c r="E169" t="n">
+        <v>18.25712776184082</v>
+      </c>
+      <c r="F169" t="n">
+        <v>-23.42814636230469</v>
+      </c>
+      <c r="G169" t="n">
+        <v>-50.89119338989258</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="B170" t="n">
+        <v>24.404436</v>
+      </c>
+      <c r="C170" t="n">
+        <v>1188.461669921875</v>
+      </c>
+      <c r="D170" t="n">
+        <v>-69.20090484619141</v>
+      </c>
+      <c r="E170" t="n">
+        <v>19.48752212524414</v>
+      </c>
+      <c r="F170" t="n">
+        <v>-22.42019462585449</v>
+      </c>
+      <c r="G170" t="n">
+        <v>-43.84865951538086</v>
       </c>
     </row>
   </sheetData>

</xml_diff>